<commit_message>
Finish tests about graph search algorithms close #11
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Logical/Test_GraphSearchAlgorithms.xlsx
+++ b/Documentation/Tests/Logical/Test_GraphSearchAlgorithms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\LAPR5\Documentation\Tests\Artificial Intelligence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\LAPR5\Documentation\Tests\Logical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Area</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>L=['JoseCid','Francisco','Diogo','Tiago','Stephanie','Maria']</t>
+  </si>
+  <si>
+    <t>L=['Simao','Joao','Tiago','Diogo','Stephanie','Maria']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Joao','Marcia',L)</t>
+  </si>
+  <si>
+    <t>L=['Joao','Artur','Andre','Tiago','Marcia']</t>
   </si>
 </sst>
 </file>
@@ -215,11 +224,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Cor3" xfId="1" builtinId="37"/>
@@ -292,8 +302,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B9:E25" totalsRowShown="0">
-  <autoFilter ref="B9:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B9:E30" totalsRowShown="0">
+  <autoFilter ref="B9:E30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Coluna1"/>
     <tableColumn id="2" name="Coluna2"/>
@@ -567,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:E32"/>
+  <dimension ref="B9:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,14 +811,56 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>